<commit_message>
Kolom verwijderd uit Excelbestand
</commit_message>
<xml_diff>
--- a/bestanden/Familiebestand.xlsx
+++ b/bestanden/Familiebestand.xlsx
@@ -1,42 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projecten\Python\excelLezenEnSchrijven\bestanden\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF7728F-EC09-48E5-AEF6-7415B024A138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5670" yWindow="2670" windowWidth="18000" windowHeight="9360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="5670" yWindow="2670" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Voorblad" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Familie" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Voorblad" sheetId="1" r:id="rId1"/>
+    <sheet name="Familie" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>Dit is het voorblad</t>
+  </si>
+  <si>
+    <t>Naam</t>
+  </si>
+  <si>
+    <t>Verband</t>
+  </si>
+  <si>
+    <t>Geboortedatum</t>
+  </si>
+  <si>
+    <t>Jaapje</t>
+  </si>
+  <si>
+    <t>Broer</t>
+  </si>
+  <si>
+    <t>Joopje</t>
+  </si>
+  <si>
+    <t>Joepje</t>
+  </si>
+  <si>
+    <t>Abraham</t>
+  </si>
+  <si>
+    <t>Vader</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,82 +95,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,27 +411,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="17.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Dit is het voorblad</t>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -459,121 +432,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="16.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="15.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="2">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Naam</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Verband</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Geboortedatum</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Leeftijd</t>
-        </is>
-      </c>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1"/>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Jaapje</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Broer</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
         <v>21961</v>
       </c>
-      <c r="D2" t="n">
-        <v>60</v>
-      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Joopje</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Broer</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
         <v>22721</v>
       </c>
-      <c r="D3" t="n">
-        <v>58</v>
-      </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Joepje</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Broer</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
         <v>23484</v>
       </c>
-      <c r="D4" t="n">
-        <v>56</v>
-      </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Abraham</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Vader</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
         <v>8765</v>
-      </c>
-      <c r="D5" t="n">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bestanden toegevoegd aan lijst met te negeren bestanden.
</commit_message>
<xml_diff>
--- a/bestanden/Familiebestand.xlsx
+++ b/bestanden/Familiebestand.xlsx
@@ -1,82 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projecten\Python\excelLezenEnSchrijven\bestanden\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF7728F-EC09-48E5-AEF6-7415B024A138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="2670" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5670" yWindow="2670" windowWidth="18000" windowHeight="9360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Voorblad" sheetId="1" r:id="rId1"/>
-    <sheet name="Familie" sheetId="2" r:id="rId2"/>
+    <sheet name="Voorblad" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Familie" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>Dit is het voorblad</t>
-  </si>
-  <si>
-    <t>Naam</t>
-  </si>
-  <si>
-    <t>Verband</t>
-  </si>
-  <si>
-    <t>Geboortedatum</t>
-  </si>
-  <si>
-    <t>Jaapje</t>
-  </si>
-  <si>
-    <t>Broer</t>
-  </si>
-  <si>
-    <t>Joopje</t>
-  </si>
-  <si>
-    <t>Joepje</t>
-  </si>
-  <si>
-    <t>Abraham</t>
-  </si>
-  <si>
-    <t>Vader</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -95,23 +55,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -411,19 +430,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col width="17.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Dit is het voorblad</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -432,7 +459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -442,69 +473,107 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="16.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1"/>
+    <row r="1" customFormat="1" s="2">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Naam</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Verband</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Geboortedatum</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Leeftijd</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Jaapje</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Broer</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>21961</v>
       </c>
+      <c r="D2" t="n">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Joopje</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Broer</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>22721</v>
       </c>
+      <c r="D3" t="n">
+        <v>58</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Joepje</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Broer</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>23484</v>
       </c>
+      <c r="D4" t="n">
+        <v>56</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Abraham</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Vader</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>8765</v>
+      </c>
+      <c r="D5" t="n">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>